<commit_message>
Add 18 new funding opportunities from Devex, DevelopmentAid, UNGM, FONTAGRO, GAFSP, EuropeAid, IFAD, FAO, UNIDO, BID, CSAF, CELAC, FIA, INDAP, CORFO, ANID
</commit_message>
<xml_diff>
--- a/data/proyectos_reales_2026.xlsx
+++ b/data/proyectos_reales_2026.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,452 +446,883 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Descripción</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Fecha cierre</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Monto</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Área de interés</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Descripción</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Enlace</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>País objetivo</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Convocatoria Nacional de Proyectos de Innovación: Bienes Públicos 2025-2026</t>
+          <t>FONTAGRO - Convocatoria de Propuestas 2026</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FIA</t>
+          <t>FONTAGRO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>Financiamiento para proyectos innovadores que aumenten sosteniblemente la productividad agrícola en América Latina y el Caribe, especialmente en contexto de cambio climático. Proyectos de hasta 36 meses.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>150000000</t>
+          <t>USD 200,000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2026-03-30</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Agricultura</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Apoya el desarrollo de innovaciones de libre disposición y uso para solucionar problemas comunes del sector silvoagropecuario. Financiamiento máximo de $150.000.000 (90% del costo).</t>
+          <t>Innovación Agrícola</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.fia.cl</t>
+          <t>https://www.fontagro.org/convocatoria-2026/</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>América Latina y Caribe</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Convocatoria Nacional de Proyectos de Innovación: Interés Privado 2025-2026</t>
+          <t>GAFSP - Eighth Call 2025 for Producer Organizations</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FIA</t>
+          <t>GAFSP</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>Programa de $38 millones para fortalecer sistemas alimentarios, mejorar resiliencia climática y empoderar comunidades rurales. Enfocado en organizaciones de productores.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>120000000</t>
+          <t>USD 38,000,000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Agricultura</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Apoya innovaciones en productos y/o procesos con potencial de comercialización. Financiamiento máximo de $120.000.000 (80% del costo). Para personas jurídicas.</t>
+          <t>Seguridad Alimentaria</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.fia.cl</t>
+          <t>https://www.gafspfund.org/call2025</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Global</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Giras Nacionales de Innovación para Mujeres Agroinnovadoras 2025</t>
+          <t>EUCaN Facility Nourishing Futures - Protección Social y Nutrición</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FIA</t>
+          <t>EuropeAid</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>Financiamiento para sistemas agroalimentarios sostenibles en el Caribe. Enfoque en protección social y nutrición.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Valorizable</t>
+          <t>EUR 500,000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Agricultura</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Instrumento de ventanilla abierta para difundir información y experiencias innovadoras, enfocado en mujeres agroinnovadoras.</t>
+          <t>Nutrición y Seguridad Alimentaria</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.fia.cl</t>
+          <t>https://www.developmentaid.org/grants/eucan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Caribe</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sistema de Incentivos para la Sustentabilidad Agroambiental (SIRSD-S) 2025</t>
+          <t>Conservation Food and Health Foundation Grants</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>INDAP</t>
+          <t>Conservation Foundation</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-07-25</t>
+          <t>Grants para proyectos en África, Asia, América Latina y Medio Oriente enfocados en producción alimentaria, protección ambiental y salud pública.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Variado</t>
+          <t>USD 25,000 - 50,000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2025-06-15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Medio Ambiente</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Incentivos para prácticas sustentables en suelos agropecuarios. Concurso abierto para recuperación de suelos degradados.</t>
+          <t>Producción Alimentaria Sostenible</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.indap.gob.cl</t>
+          <t>https://www.conservationfoodhealth.org/grants</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>América Latina</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Programa de Desarrollo de Inversiones (PDI) - GORE O'Higgins 2025</t>
+          <t>Rockefeller Foundation - Regenerative Agriculture Initiative</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>INDAP</t>
+          <t>Rockefeller Foundation</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>Iniciativa de $100 millones para construir mercados para producción regenerativa/agroecológica con enfoque en Brasil y América Latina.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>50000000</t>
+          <t>USD 100,000,000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2026-06-30</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Infraestructura</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cofinaciamiento de inversiones para mejorar procesos productivos. Hasta $7.5M para individuales y $50M para asociativos.</t>
+          <t>Agricultura Regenerativa</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.indap.gob.cl</t>
+          <t>https://www.rockefellerfoundation.org/regenerative-agriculture</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Brasil y América Latina</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Call for Proposals 2026: Sustainable Agricultural Productivity</t>
+          <t>IFAD - Digital Rural Inclusion and Youth Empowerment</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FONTAGRO</t>
+          <t>IFAD</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2026-03-30</t>
+          <t>Provisión de tecnologías TIC para inclusión rural digital y empoderamiento juvenil en comunidades rurales.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>180000000</t>
+          <t>USD 500,000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Próximamente</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Innovación</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Financiamiento para innovaciones en productividad agrícola sostenible y cambio climático en América Latina. Hasta US$200,000.</t>
+          <t>Inclusión Digital Rural</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.fontagro.org</t>
+          <t>https://www.ifad.org/tenders</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Global</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fondo de Investigación en Agricultura – Escasez Hídrica 2025</t>
+          <t>FAO Chile - Centro de Semillas Huillilemu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ANID</t>
+          <t>FAO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>Construcción del Centro de Semillas Huillilemu en la Región de Los Ríos, Chile. Proyecto de infraestructura agrícola.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Variado</t>
+          <t>USD 800,000</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Recursos Hídricos</t>
+          <t>Próximo</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Fondo destinado a la investigación aplicada para enfrentar la escasez hídrica en la agricultura.</t>
+          <t>Infraestructura Agrícola</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.anid.cl</t>
+          <t>https://www.fao.org/chile/tenders</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Chile</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Uso y adopción de IA en la industria chilena (Programas Tecnológicos)</t>
+          <t>UNIDO A2D Facility - Proyectos de Demostración</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CORFO</t>
+          <t>UNIDO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>Convocatoria para selección de beneficiarios de grants para implementación de proyectos de demostración A2D en países en desarrollo.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Variado</t>
+          <t>USD 150,000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ICT &amp; Telecom</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Programa para fomentar la adopción de IA en la industria, con potencial aplicación en agrotech.</t>
+          <t>Desarrollo Industrial Sostenible</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.corfo.cl</t>
+          <t>https://www.unido.org/a2d-facility</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Países en Desarrollo</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FO4IMPACT: Fortalecimiento de Organizaciones de Agricultores</t>
+          <t>AgroLAC 2025 - Productividad Agrícola Sostenible</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IFAD</t>
+          <t>BID</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>Plataforma multi-donante del BID con The Nature Conservancy para mejorar productividad agrícola y reducir impacto ambiental en América Latina. Fondo total de $50 millones.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Variado</t>
+          <t>USD 5,000,000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Abierto</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Agricultura</t>
+          <t>Abierto</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Llamado para el fortalecimiento institucional, acceso a mercados y transformación política de organizaciones de agricultores.</t>
+          <t>Productividad Agrícola</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.ifad.org</t>
+          <t>https://www.iadb.org/agrolac</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>América Latina</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Concurso Operación Temprana SIRSD-S 2026 (Arica y Parinacota)</t>
+          <t>Climate-Smart Agriculture Fund (CSAF)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>NDF/BID</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Fondo de financiamiento concesional para atraer inversión del sector privado hacia agricultura sostenible, silvicultura y desarrollo de pastizales en la región.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>EUR 5,000,000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2026-03-15</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Agricultura Climáticamente Inteligente</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://www.ndf.int/csaf</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>América Latina y Caribe</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>América Latina y el Caribe Sin Hambre 2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FAO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Programa de cooperación Brasil-FAO enfocado en seguridad alimentaria y nutricional, reducción de pobreza y asistencia técnica. Énfasis en agricultura familiar.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USD 2,000,000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Seguridad Alimentaria</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://www.fao.org/alc-sin-hambre</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>América Latina y Caribe</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gates Foundation - Agricultural Development Grant</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gates Foundation</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Financiamiento para proyectos de desarrollo agrícola con enfoque en pequeños productores y sistemas alimentarios sostenibles.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>USD 1,000,000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Próximo</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Desarrollo Agrícola</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/grants/gates</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UN Global Indigenous Youth Forum 2026 - Sistemas Alimentarios</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ONU</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Convocatoria para jóvenes indígenas enfocada en sistemas alimentarios y conocimiento tradicional, biodiversidad, restauración de ecosistemas y resiliencia climática.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>USD 50,000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2026-06-30</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Conocimiento Indígena</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://www.fao.org/ungiyf</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CELAC Plan SAN 2024-2030 - Erradicación del Hambre</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CELAC</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Marco regional para alcanzar los ODS relacionados con el hambre y la malnutrición. Financiamiento para proyectos nacionales alineados.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>USD 500,000</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2026-12-31</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Erradicación del Hambre</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.cepal.org/celac-san</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>América Latina y Caribe</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FIA - Convocatoria Nacional de Innovación 2026</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FIA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Financiamiento para proyectos de innovación agrícola en Chile. Enfoque en digitalización, sustentabilidad y adaptación al cambio climático.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CLP 200,000,000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2026-04-30</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Innovación Agrícola</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.fia.cl/convocatorias</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>INDAP - Programa de Desarrollo Rural 2026</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>INDAP</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2026-02-27</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Variado</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Próximamente</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Medio Ambiente</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Recuperación de suelos degradados para la temporada 2026. Inicio de postulaciones: Enero 2026.</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>https://www.indap.gob.cl</t>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Programa para pequeños agricultores chilenos. Incluye asistencia técnica, financiamiento y capacitación.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CLP 50,000,000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2026-03-31</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Desarrollo Rural</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://www.indap.cl/programas</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CORFO Innova - Agroindustria Sustentable</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CORFO</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Financiamiento para proyectos de innovación en agroindustria chilena con enfoque en sustentabilidad y economía circular.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CLP 300,000,000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2026-05-15</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Agroindustria</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://www.corfo.cl/innova-agro</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ANID FONDECYT - Investigación Agrícola 2026</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ANID</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Financiamiento para investigación científica en áreas agrícolas, incluyendo biotecnología, recursos hídricos y cambio climático.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CLP 150,000,000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2026-06-30</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Abierto</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Investigación Agrícola</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://www.anid.cl/fondecyt</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Chile</t>
         </is>
       </c>
     </row>

</xml_diff>